<commit_message>
[Develop] The task list was updated
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -70,9 +70,6 @@
     <t>9. Feature to download/upload list of words</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Arthur</t>
   </si>
   <si>
@@ -83,6 +80,12 @@
   </si>
   <si>
     <t>12. Feature to search the most "red" news</t>
+  </si>
+  <si>
+    <t>Upload feature remained</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -676,14 +679,15 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -709,9 +713,11 @@
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -805,15 +811,15 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>10</v>
@@ -825,7 +831,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>5</v>
@@ -837,7 +843,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
[Develop] The task list was changed
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -85,14 +85,20 @@
     <t>Upload feature remained</t>
   </si>
   <si>
-    <t>In progress</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>13. Fix bug of incorrect div count</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +115,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -363,7 +377,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -372,6 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -679,7 +693,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,16 +706,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -709,13 +723,13 @@
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -723,7 +737,7 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -735,7 +749,7 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -747,7 +761,7 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -759,19 +773,21 @@
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -783,7 +799,7 @@
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -795,7 +811,7 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -807,7 +823,7 @@
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -821,7 +837,7 @@
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -833,7 +849,7 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -845,7 +861,7 @@
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -854,50 +870,56 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="15"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="15"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="15"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
     </row>

</xml_diff>

<commit_message>
[Develop] The list of tasks was updated.
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -715,7 +715,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -890,8 +890,8 @@
       <c r="B13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
+      <c r="C13" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
[Develop] Quick style fixes
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -101,16 +101,13 @@
   </si>
   <si>
     <t>17. Add links to sites</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,14 +140,6 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -396,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -416,7 +405,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -724,7 +712,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,8 +943,8 @@
       <c r="B17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>29</v>
+      <c r="C17" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
[Develop] Some style fixes were made
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>17. Add links to sites</t>
+  </si>
+  <si>
+    <t>18. Change colour of underlined words</t>
+  </si>
+  <si>
+    <t>19. Make feature to add word to ban list by clicking</t>
   </si>
 </sst>
 </file>
@@ -712,7 +718,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,15 +969,29 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Separate_menus] The menu settings were separated.
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>19. Make feature to add word to ban list by clicking</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -718,7 +721,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,9 +769,11 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -869,10 +874,12 @@
       <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3"/>
+      <c r="C11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">

</xml_diff>

<commit_message>
[Add_list_of_links] The list was added.
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>19. Make feature to add word to ban list by clicking</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -721,7 +718,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>18</v>
@@ -970,8 +967,8 @@
       <c r="B18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
+      <c r="C18" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="D18" s="3"/>
     </row>

</xml_diff>

<commit_message>
[Ad_review_page] The review page was added but not fully implemented.
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -107,6 +107,21 @@
   </si>
   <si>
     <t>19. Make feature to add word to ban list by clicking</t>
+  </si>
+  <si>
+    <t>20. Add review page</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>21. Change settings address (licence, word list) to my documents</t>
+  </si>
+  <si>
+    <t>22. Add feature to calculate new news on the sites</t>
+  </si>
+  <si>
+    <t>23. Add feature to calculate new added by user</t>
   </si>
 </sst>
 </file>
@@ -715,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,27 +1014,53 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,13 +1075,103 @@
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Develop] The feature to add news to site was added.
</commit_message>
<xml_diff>
--- a/Documentation/TaskList.xlsx
+++ b/Documentation/TaskList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
   <si>
     <t>Task</t>
   </si>
@@ -106,9 +106,6 @@
     <t>18. Change colour of underlined words</t>
   </si>
   <si>
-    <t>19. Make feature to add word to ban list by clicking</t>
-  </si>
-  <si>
     <t>20. Add review page</t>
   </si>
   <si>
@@ -119,6 +116,15 @@
   </si>
   <si>
     <t>23. Add feature to calculate new added by user</t>
+  </si>
+  <si>
+    <t>24. Add feature to make chance to change data in the time of review</t>
+  </si>
+  <si>
+    <t>19. Make feature to add word to ban list by clicking ( + change colour of words)</t>
+  </si>
+  <si>
+    <t>25. Update algorithm to find data by using {0}{1}..{n} markers</t>
   </si>
 </sst>
 </file>
@@ -721,7 +727,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +1001,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>10</v>
@@ -1007,7 +1013,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>8</v>
@@ -1021,7 +1027,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>5</v>
@@ -1033,7 +1039,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>5</v>
@@ -1045,7 +1051,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>5</v>
@@ -1056,15 +1062,27 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>